<commit_message>
version 2 of the dockerization of DataCatalogue
</commit_message>
<xml_diff>
--- a/src/main/resources/data/ErrorFiles/dementia_Niguarda_v2.xlsx
+++ b/src/main/resources/data/ErrorFiles/dementia_Niguarda_v2.xlsx
@@ -624,7 +624,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:M38"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -791,7 +791,7 @@
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>

</xml_diff>